<commit_message>
Made progress report 5
</commit_message>
<xml_diff>
--- a/Document/Worklogs(NEn408).xlsx
+++ b/Document/Worklogs(NEn408).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://collegedouglas-my.sharepoint.com/personal/enkhbatn_student_douglascollege_ca/Documents/1. DCI/6. 2025 Fall/CSIS 4495 Applied research/Git/HealthAcademyNen08/F2025_4495_050_Nen408/Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="11_F25DC773A252ABDACC10485461DD4EB45BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F46159CC-0925-462D-B1C2-393E634CB3E0}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="11_F25DC773A252ABDACC10485461DD4EB45BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F26C0E22-C332-41B0-91CD-869DAF49E218}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -48,9 +48,6 @@
     <t>we received the files and got admin for wordpress, I run health academy website, tried to connect existing chatbot, but it seems not working well, I will look for another way</t>
   </si>
   <si>
-    <t>https://github.com/narkmn/HealthAcademyNen08</t>
-  </si>
-  <si>
     <t>Tested chatbot</t>
   </si>
   <si>
@@ -112,6 +109,27 @@
   </si>
   <si>
     <t>Testing on removing unnecessary plugins and pages, Removed 4 plugin and it worked okay</t>
+  </si>
+  <si>
+    <t>Improved migration code, because of database url problem, I created 3 migration scripts.</t>
+  </si>
+  <si>
+    <t>Researched openai chatbot, and custom plugin of wordpress</t>
+  </si>
+  <si>
+    <t>Tested editing custom plugin in www.dataofattraction.com, however something is broken, now I cannot access use customize tool</t>
+  </si>
+  <si>
+    <t>Created AI chatbot plugin in local wordpress host. It is working fine, but it work like Chatgpt, not personalized and related to topic</t>
+  </si>
+  <si>
+    <t>AI chatbot</t>
+  </si>
+  <si>
+    <t>added the plugin into healthcare.ca and localhost. And get user info and saved chat history in database. Added last 10 chat history along with all class topic since there is no way which class student in</t>
+  </si>
+  <si>
+    <t>https://github.com/narkmn/F2025_4495_050_Nen408</t>
   </si>
 </sst>
 </file>
@@ -227,6 +245,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -495,10 +517,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +533,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -553,7 +575,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>6</v>
@@ -567,10 +589,10 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -581,10 +603,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
@@ -595,10 +617,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -609,10 +631,10 @@
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -623,10 +645,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -637,10 +659,10 @@
         <v>2</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -651,10 +673,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -665,10 +687,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -679,10 +701,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -693,10 +715,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -707,10 +729,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -721,10 +743,10 @@
         <v>2</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -735,10 +757,10 @@
         <v>6.5</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -749,10 +771,80 @@
         <v>2</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="3">
+        <v>45970</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="3">
+        <v>45970</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B22" s="3">
+        <v>45974</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B23" s="3">
+        <v>45975</v>
+      </c>
+      <c r="C23" s="2">
+        <v>6</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="3">
+        <v>45976</v>
+      </c>
+      <c r="C24" s="2">
+        <v>6</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -760,9 +852,9 @@
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" xr:uid="{3B05DAF9-EB44-448E-B265-8D6148DAF9FD}"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{1A6D7137-B595-42D6-9623-BC190AC7B4EC}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
+  <pageSetup scale="88" orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>